<commit_message>
[AircraftPointPropagation] Test01 in Sandbox2.atsi.analyses.test1
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/ATR-72 - ATsi/BALANCE/Balance.xlsx
+++ b/JPADSandBox_v2/out/ATR-72 - ATsi/BALANCE/Balance.xlsx
@@ -256,10 +256,10 @@
     <t>Xcg ESTIMATION METHOD COMPARISON (WITHOUT CALIBRATIONS)</t>
   </si>
   <si>
+    <t>TORENBEEK_1982</t>
+  </si>
+  <si>
     <t>SFORZA</t>
-  </si>
-  <si>
-    <t>TORENBEEK_1982</t>
   </si>
   <si>
     <t>Ycg LRF (semi-wing)</t>
@@ -1251,7 +1251,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>11.500334910927485</v>
+        <v>10.594739999999998</v>
       </c>
     </row>
     <row r="24">
@@ -1262,7 +1262,7 @@
         <v>5</v>
       </c>
       <c r="C24" t="n">
-        <v>10.594739999999998</v>
+        <v>11.500334910927485</v>
       </c>
     </row>
   </sheetData>
@@ -1502,7 +1502,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>0.8092048979331106</v>
+        <v>1.133712717373045</v>
       </c>
     </row>
     <row r="24">
@@ -1513,7 +1513,7 @@
         <v>5</v>
       </c>
       <c r="C24" t="n">
-        <v>1.133712717373045</v>
+        <v>0.8092048979331106</v>
       </c>
     </row>
     <row r="25">
@@ -1534,7 +1534,7 @@
         <v>5</v>
       </c>
       <c r="C27" t="n">
-        <v>10.850510037388545</v>
+        <v>5.087959999999999</v>
       </c>
     </row>
     <row r="28">
@@ -1545,7 +1545,7 @@
         <v>5</v>
       </c>
       <c r="C28" t="n">
-        <v>5.087959999999999</v>
+        <v>10.850510037388545</v>
       </c>
     </row>
   </sheetData>
@@ -2003,7 +2003,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -2024,7 +2024,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
@@ -2264,7 +2264,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -2285,7 +2285,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
@@ -2765,7 +2765,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -3005,7 +3005,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -3026,7 +3026,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
New test #01 in Sandbox 2 - ATsi
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/ATR-72 - ATsi/BALANCE/Balance.xlsx
+++ b/JPADSandBox_v2/out/ATR-72 - ATsi/BALANCE/Balance.xlsx
@@ -382,7 +382,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="n">
-        <v>12.191162919778115</v>
+        <v>12.141605723464071</v>
       </c>
     </row>
     <row r="4">
@@ -404,7 +404,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="n">
-        <v>0.11524794485395798</v>
+        <v>0.1170958407255597</v>
       </c>
     </row>
     <row r="6">
@@ -420,7 +420,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="n">
-        <v>49.83250922882285</v>
+        <v>48.8697450578075</v>
       </c>
     </row>
     <row r="8">
@@ -442,7 +442,7 @@
         <v>10</v>
       </c>
       <c r="C9" t="n">
-        <v>4.760625171259168</v>
+        <v>5.046722739735554</v>
       </c>
     </row>
     <row r="10">
@@ -468,7 +468,7 @@
         <v>5</v>
       </c>
       <c r="C13" t="n">
-        <v>11.82398098424618</v>
+        <v>11.785103940501518</v>
       </c>
     </row>
     <row r="14">
@@ -490,7 +490,7 @@
         <v>5</v>
       </c>
       <c r="C15" t="n">
-        <v>0.26437248358866916</v>
+        <v>0.265163019047306</v>
       </c>
     </row>
     <row r="16">
@@ -506,7 +506,7 @@
         <v>10</v>
       </c>
       <c r="C17" t="n">
-        <v>34.6650755106766</v>
+        <v>33.50484700775513</v>
       </c>
     </row>
     <row r="18">
@@ -528,7 +528,7 @@
         <v>10</v>
       </c>
       <c r="C19" t="n">
-        <v>10.9206138257423</v>
+        <v>11.428281565519924</v>
       </c>
     </row>
     <row r="20">
@@ -554,7 +554,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>11.82398098424618</v>
+        <v>11.785103940501518</v>
       </c>
     </row>
     <row r="24">
@@ -576,7 +576,7 @@
         <v>5</v>
       </c>
       <c r="C25" t="n">
-        <v>0.26437248358866916</v>
+        <v>0.265163019047306</v>
       </c>
     </row>
     <row r="26">
@@ -592,7 +592,7 @@
         <v>10</v>
       </c>
       <c r="C27" t="n">
-        <v>34.6650755106766</v>
+        <v>33.50484700775513</v>
       </c>
     </row>
     <row r="28">
@@ -614,7 +614,7 @@
         <v>10</v>
       </c>
       <c r="C29" t="n">
-        <v>10.9206138257423</v>
+        <v>11.428281565519924</v>
       </c>
     </row>
     <row r="30">
@@ -640,7 +640,7 @@
         <v>5</v>
       </c>
       <c r="C33" t="n">
-        <v>11.82398098424618</v>
+        <v>11.785103940501518</v>
       </c>
     </row>
     <row r="34">
@@ -662,7 +662,7 @@
         <v>5</v>
       </c>
       <c r="C35" t="n">
-        <v>0.26437248358866916</v>
+        <v>0.265163019047306</v>
       </c>
     </row>
     <row r="36">
@@ -678,7 +678,7 @@
         <v>10</v>
       </c>
       <c r="C37" t="n">
-        <v>34.6650755106766</v>
+        <v>33.50484700775513</v>
       </c>
     </row>
     <row r="38">
@@ -700,7 +700,7 @@
         <v>10</v>
       </c>
       <c r="C39" t="n">
-        <v>10.9206138257423</v>
+        <v>11.428281565519924</v>
       </c>
     </row>
     <row r="40">
@@ -726,7 +726,7 @@
         <v>5</v>
       </c>
       <c r="C43" t="n">
-        <v>12.002801810951546</v>
+        <v>11.97639295538773</v>
       </c>
     </row>
     <row r="44">
@@ -748,7 +748,7 @@
         <v>5</v>
       </c>
       <c r="C45" t="n">
-        <v>0.17950228112805888</v>
+        <v>0.1802658333969227</v>
       </c>
     </row>
     <row r="46">
@@ -764,7 +764,7 @@
         <v>10</v>
       </c>
       <c r="C47" t="n">
-        <v>42.05174891155756</v>
+        <v>41.74922712669088</v>
       </c>
     </row>
     <row r="48">
@@ -786,7 +786,7 @@
         <v>10</v>
       </c>
       <c r="C49" t="n">
-        <v>7.4148227017805155</v>
+        <v>7.769291163243255</v>
       </c>
     </row>
     <row r="50">
@@ -812,7 +812,7 @@
         <v>5</v>
       </c>
       <c r="C53" t="n">
-        <v>11.989289361632132</v>
+        <v>11.963789830651873</v>
       </c>
     </row>
     <row r="54">
@@ -834,7 +834,7 @@
         <v>5</v>
       </c>
       <c r="C55" t="n">
-        <v>0.44754789626086433</v>
+        <v>0.46880783296563133</v>
       </c>
     </row>
     <row r="56">
@@ -850,7 +850,7 @@
         <v>10</v>
       </c>
       <c r="C57" t="n">
-        <v>41.49358098555356</v>
+        <v>41.20604407422656</v>
       </c>
     </row>
     <row r="58">
@@ -872,7 +872,7 @@
         <v>10</v>
       </c>
       <c r="C59" t="n">
-        <v>18.487165068179394</v>
+        <v>20.20518522719279</v>
       </c>
     </row>
     <row r="60">
@@ -893,7 +893,7 @@
         <v>10</v>
       </c>
       <c r="C62" t="n">
-        <v>20.340187707059705</v>
+        <v>18.778612969176336</v>
       </c>
     </row>
     <row r="63">
@@ -904,7 +904,7 @@
         <v>10</v>
       </c>
       <c r="C63" t="n">
-        <v>41.49358098555356</v>
+        <v>41.20604407422656</v>
       </c>
     </row>
     <row r="64">
@@ -915,7 +915,7 @@
         <v>10</v>
       </c>
       <c r="C64" t="n">
-        <v>54.24025116750932</v>
+        <v>54.32676647955055</v>
       </c>
     </row>
     <row r="65">
@@ -946,7 +946,7 @@
         <v>53</v>
       </c>
       <c r="C69" t="n">
-        <v>45821.44336009229</v>
+        <v>47870.72870372752</v>
       </c>
     </row>
     <row r="70">
@@ -957,7 +957,7 @@
         <v>53</v>
       </c>
       <c r="C70" t="n">
-        <v>750311.9952829664</v>
+        <v>745048.6735852612</v>
       </c>
     </row>
     <row r="71">
@@ -968,7 +968,7 @@
         <v>53</v>
       </c>
       <c r="C71" t="n">
-        <v>704490.5519228742</v>
+        <v>697177.9448815337</v>
       </c>
     </row>
     <row r="72">
@@ -1011,7 +1011,7 @@
         <v>53</v>
       </c>
       <c r="C76" t="n">
-        <v>48619.36661211877</v>
+        <v>48532.61138617322</v>
       </c>
     </row>
   </sheetData>
@@ -1077,7 +1077,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>2.591995059072891</v>
+        <v>1.7164117478640433</v>
       </c>
     </row>
     <row r="6">
@@ -1088,7 +1088,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="n">
-        <v>2.591995059072854</v>
+        <v>1.7164117478640046</v>
       </c>
     </row>
     <row r="7">
@@ -1328,7 +1328,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>32.49550627232441</v>
+        <v>33.26255957187139</v>
       </c>
     </row>
     <row r="6">
@@ -1339,7 +1339,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="n">
-        <v>32.49550627232441</v>
+        <v>33.26255957187139</v>
       </c>
     </row>
     <row r="7">
@@ -1350,7 +1350,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>0.9714588076530777</v>
+        <v>0.9794823019718901</v>
       </c>
     </row>
     <row r="8">
@@ -1361,7 +1361,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="n">
-        <v>0.9714588076530777</v>
+        <v>0.9794823019718901</v>
       </c>
     </row>
     <row r="9">
@@ -1372,7 +1372,7 @@
         <v>5</v>
       </c>
       <c r="C9" t="n">
-        <v>11.771458807653076</v>
+        <v>11.779482301971889</v>
       </c>
     </row>
     <row r="10">
@@ -1383,7 +1383,7 @@
         <v>5</v>
       </c>
       <c r="C10" t="n">
-        <v>11.771458807653076</v>
+        <v>11.779482301971889</v>
       </c>
     </row>
     <row r="11">
@@ -1399,7 +1399,7 @@
         <v>5</v>
       </c>
       <c r="C12" t="n">
-        <v>5.087959999999999</v>
+        <v>5.409999999999998</v>
       </c>
     </row>
     <row r="13">
@@ -1410,7 +1410,7 @@
         <v>5</v>
       </c>
       <c r="C13" t="n">
-        <v>5.087959999999998</v>
+        <v>5.4099999999999975</v>
       </c>
     </row>
     <row r="14">
@@ -1426,7 +1426,7 @@
         <v>10</v>
       </c>
       <c r="C15" t="n">
-        <v>66.09228723051781</v>
+        <v>68.95852434675184</v>
       </c>
     </row>
     <row r="16">
@@ -1437,7 +1437,7 @@
         <v>10</v>
       </c>
       <c r="C16" t="n">
-        <v>66.09228723051781</v>
+        <v>68.95852434675184</v>
       </c>
     </row>
     <row r="17">
@@ -1502,7 +1502,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>1.133712717373045</v>
+        <v>1.104420538817831</v>
       </c>
     </row>
     <row r="24">
@@ -1513,7 +1513,7 @@
         <v>5</v>
       </c>
       <c r="C24" t="n">
-        <v>0.8092048979331106</v>
+        <v>0.8545440651259495</v>
       </c>
     </row>
     <row r="25">
@@ -1534,7 +1534,7 @@
         <v>5</v>
       </c>
       <c r="C27" t="n">
-        <v>5.087959999999999</v>
+        <v>5.409999999999998</v>
       </c>
     </row>
     <row r="28">
@@ -1545,7 +1545,7 @@
         <v>5</v>
       </c>
       <c r="C28" t="n">
-        <v>10.850510037388545</v>
+        <v>10.998778735632179</v>
       </c>
     </row>
   </sheetData>
@@ -1611,7 +1611,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>39.09375884989063</v>
+        <v>39.07656408472137</v>
       </c>
     </row>
     <row r="6">
@@ -1622,7 +1622,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="n">
-        <v>39.093758849890584</v>
+        <v>39.07656408472133</v>
       </c>
     </row>
     <row r="7">
@@ -1633,7 +1633,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>1.1311930908272143</v>
+        <v>1.1143808849778667</v>
       </c>
     </row>
     <row r="8">
@@ -1644,7 +1644,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="n">
-        <v>1.1311930908272143</v>
+        <v>1.1143808849778667</v>
       </c>
     </row>
     <row r="9">
@@ -1655,7 +1655,7 @@
         <v>5</v>
       </c>
       <c r="C9" t="n">
-        <v>11.931193090827213</v>
+        <v>11.914380884977867</v>
       </c>
     </row>
     <row r="10">
@@ -1666,7 +1666,7 @@
         <v>5</v>
       </c>
       <c r="C10" t="n">
-        <v>11.931193090827211</v>
+        <v>11.914380884977865</v>
       </c>
     </row>
     <row r="11">
@@ -1709,7 +1709,7 @@
         <v>10</v>
       </c>
       <c r="C15" t="n">
-        <v>66.09228723051781</v>
+        <v>68.95852434675184</v>
       </c>
     </row>
     <row r="16">
@@ -1720,7 +1720,7 @@
         <v>10</v>
       </c>
       <c r="C16" t="n">
-        <v>66.0922872305178</v>
+        <v>68.95852434675184</v>
       </c>
     </row>
     <row r="17">
@@ -1835,7 +1835,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>627.8510862041463</v>
+        <v>654.0912358990008</v>
       </c>
     </row>
     <row r="6">
@@ -1846,7 +1846,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="n">
-        <v>627.8510862041463</v>
+        <v>654.0912358990008</v>
       </c>
     </row>
     <row r="7">
@@ -1933,7 +1933,7 @@
         <v>10</v>
       </c>
       <c r="C15" t="n">
-        <v>236.998680472733</v>
+        <v>247.27664849190882</v>
       </c>
     </row>
     <row r="16">
@@ -1944,7 +1944,7 @@
         <v>10</v>
       </c>
       <c r="C16" t="n">
-        <v>236.998680472733</v>
+        <v>247.27664849190882</v>
       </c>
     </row>
     <row r="17">
@@ -2096,7 +2096,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>561.1310506278867</v>
+        <v>584.4777395215115</v>
       </c>
     </row>
     <row r="6">
@@ -2107,7 +2107,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="n">
-        <v>561.1310506278867</v>
+        <v>584.4777395215115</v>
       </c>
     </row>
     <row r="7">
@@ -2194,7 +2194,7 @@
         <v>10</v>
       </c>
       <c r="C15" t="n">
-        <v>53.699983374795714</v>
+        <v>56.028801031735874</v>
       </c>
     </row>
     <row r="16">
@@ -2205,7 +2205,7 @@
         <v>10</v>
       </c>
       <c r="C16" t="n">
-        <v>53.699983374795714</v>
+        <v>56.028801031735874</v>
       </c>
     </row>
     <row r="17">
@@ -2357,7 +2357,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>7.031023409080806</v>
+        <v>6.347948306468693</v>
       </c>
     </row>
     <row r="6">
@@ -2368,7 +2368,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="n">
-        <v>7.031023409080806</v>
+        <v>6.347948306468693</v>
       </c>
     </row>
     <row r="7">
@@ -2455,7 +2455,7 @@
         <v>10</v>
       </c>
       <c r="C15" t="n">
-        <v>38.920095642871175</v>
+        <v>40.6079510246935</v>
       </c>
     </row>
     <row r="16">
@@ -2466,7 +2466,7 @@
         <v>10</v>
       </c>
       <c r="C16" t="n">
-        <v>38.920095642871175</v>
+        <v>40.6079510246935</v>
       </c>
     </row>
     <row r="17">
@@ -2597,7 +2597,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>-34.27665610999282</v>
+        <v>-36.75112941025122</v>
       </c>
     </row>
     <row r="6">
@@ -2608,7 +2608,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="n">
-        <v>-34.27665610999282</v>
+        <v>-36.75112941025122</v>
       </c>
     </row>
     <row r="7">
@@ -2695,7 +2695,7 @@
         <v>10</v>
       </c>
       <c r="C15" t="n">
-        <v>38.920095642871175</v>
+        <v>40.6079510246935</v>
       </c>
     </row>
     <row r="16">
@@ -2706,7 +2706,7 @@
         <v>10</v>
       </c>
       <c r="C16" t="n">
-        <v>38.920095642871175</v>
+        <v>40.6079510246935</v>
       </c>
     </row>
     <row r="17">
@@ -2837,7 +2837,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>-18.416904856045285</v>
+        <v>-19.934136097328047</v>
       </c>
     </row>
     <row r="6">
@@ -2848,7 +2848,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="n">
-        <v>-18.416904856045317</v>
+        <v>-19.934136097328086</v>
       </c>
     </row>
     <row r="7">
@@ -2859,7 +2859,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>10.538941955553913</v>
+        <v>10.545193809330613</v>
       </c>
     </row>
     <row r="8">
@@ -2870,7 +2870,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="n">
-        <v>10.538941955553913</v>
+        <v>10.545193809330613</v>
       </c>
     </row>
     <row r="9">
@@ -2881,7 +2881,7 @@
         <v>5</v>
       </c>
       <c r="C9" t="n">
-        <v>10.538941955553913</v>
+        <v>10.545193809330613</v>
       </c>
     </row>
     <row r="10">
@@ -2892,7 +2892,7 @@
         <v>5</v>
       </c>
       <c r="C10" t="n">
-        <v>10.538941955553913</v>
+        <v>10.545193809330613</v>
       </c>
     </row>
     <row r="11">
@@ -2935,7 +2935,7 @@
         <v>10</v>
       </c>
       <c r="C15" t="n">
-        <v>-174.75786757557108</v>
+        <v>-186.09319776525322</v>
       </c>
     </row>
     <row r="16">
@@ -2946,7 +2946,7 @@
         <v>10</v>
       </c>
       <c r="C16" t="n">
-        <v>-174.75786757557108</v>
+        <v>-186.09319776525317</v>
       </c>
     </row>
     <row r="17">
@@ -2957,7 +2957,7 @@
         <v>5</v>
       </c>
       <c r="C17" t="n">
-        <v>-2.452638699878493</v>
+        <v>-2.5397999999999996</v>
       </c>
     </row>
     <row r="18">
@@ -2968,7 +2968,7 @@
         <v>5</v>
       </c>
       <c r="C18" t="n">
-        <v>-2.4526386998784924</v>
+        <v>-2.539799999999999</v>
       </c>
     </row>
     <row r="19">
@@ -2979,7 +2979,7 @@
         <v>5</v>
       </c>
       <c r="C19" t="n">
-        <v>-4.230638699878492</v>
+        <v>-4.317799999999999</v>
       </c>
     </row>
     <row r="20">
@@ -2990,7 +2990,7 @@
         <v>5</v>
       </c>
       <c r="C20" t="n">
-        <v>-4.230638699878492</v>
+        <v>-4.317799999999998</v>
       </c>
     </row>
     <row r="21">
@@ -3011,7 +3011,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>10.538941955553913</v>
+        <v>10.545193809330613</v>
       </c>
     </row>
     <row r="24">
@@ -3032,7 +3032,7 @@
         <v>5</v>
       </c>
       <c r="C26" t="n">
-        <v>-2.452638699878493</v>
+        <v>-2.5397999999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some work on time constant ATR72_ATsi
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/ATR-72 - ATsi/BALANCE/Balance.xlsx
+++ b/JPADSandBox_v2/out/ATR-72 - ATsi/BALANCE/Balance.xlsx
@@ -256,10 +256,10 @@
     <t>Xcg ESTIMATION METHOD COMPARISON (WITHOUT CALIBRATIONS)</t>
   </si>
   <si>
+    <t>SFORZA</t>
+  </si>
+  <si>
     <t>TORENBEEK_1982</t>
-  </si>
-  <si>
-    <t>SFORZA</t>
   </si>
   <si>
     <t>Ycg LRF (semi-wing)</t>
@@ -1251,7 +1251,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>10.594739999999998</v>
+        <v>11.500334910927485</v>
       </c>
     </row>
     <row r="24">
@@ -1262,7 +1262,7 @@
         <v>5</v>
       </c>
       <c r="C24" t="n">
-        <v>11.500334910927485</v>
+        <v>10.594739999999998</v>
       </c>
     </row>
   </sheetData>
@@ -1502,7 +1502,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>1.104420538817831</v>
+        <v>0.8545440651259495</v>
       </c>
     </row>
     <row r="24">
@@ -1513,7 +1513,7 @@
         <v>5</v>
       </c>
       <c r="C24" t="n">
-        <v>0.8545440651259495</v>
+        <v>1.104420538817831</v>
       </c>
     </row>
     <row r="25">
@@ -1534,7 +1534,7 @@
         <v>5</v>
       </c>
       <c r="C27" t="n">
-        <v>5.409999999999998</v>
+        <v>10.998778735632179</v>
       </c>
     </row>
     <row r="28">
@@ -1545,7 +1545,7 @@
         <v>5</v>
       </c>
       <c r="C28" t="n">
-        <v>10.998778735632179</v>
+        <v>5.409999999999998</v>
       </c>
     </row>
   </sheetData>
@@ -2003,7 +2003,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -2024,7 +2024,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
@@ -2264,7 +2264,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -2285,7 +2285,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
@@ -2765,7 +2765,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -3005,7 +3005,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -3026,7 +3026,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
More work on JPAD MatlabReport classes
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/ATR-72 - ATsi/BALANCE/Balance.xlsx
+++ b/JPADSandBox_v2/out/ATR-72 - ATsi/BALANCE/Balance.xlsx
@@ -256,10 +256,10 @@
     <t>Xcg ESTIMATION METHOD COMPARISON (WITHOUT CALIBRATIONS)</t>
   </si>
   <si>
+    <t>TORENBEEK_1982</t>
+  </si>
+  <si>
     <t>SFORZA</t>
-  </si>
-  <si>
-    <t>TORENBEEK_1982</t>
   </si>
   <si>
     <t>Ycg LRF (semi-wing)</t>
@@ -1251,7 +1251,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>11.500334910927485</v>
+        <v>10.594739999999998</v>
       </c>
     </row>
     <row r="24">
@@ -1262,7 +1262,7 @@
         <v>5</v>
       </c>
       <c r="C24" t="n">
-        <v>10.594739999999998</v>
+        <v>11.500334910927485</v>
       </c>
     </row>
   </sheetData>
@@ -1502,7 +1502,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>0.8545440651259495</v>
+        <v>1.104420538817831</v>
       </c>
     </row>
     <row r="24">
@@ -1513,7 +1513,7 @@
         <v>5</v>
       </c>
       <c r="C24" t="n">
-        <v>1.104420538817831</v>
+        <v>0.8545440651259495</v>
       </c>
     </row>
     <row r="25">
@@ -1534,7 +1534,7 @@
         <v>5</v>
       </c>
       <c r="C27" t="n">
-        <v>10.998778735632179</v>
+        <v>5.409999999999998</v>
       </c>
     </row>
     <row r="28">
@@ -1545,7 +1545,7 @@
         <v>5</v>
       </c>
       <c r="C28" t="n">
-        <v>5.409999999999998</v>
+        <v>10.998778735632179</v>
       </c>
     </row>
   </sheetData>
@@ -2003,7 +2003,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -2024,7 +2024,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
@@ -2264,7 +2264,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -2285,7 +2285,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
@@ -2765,7 +2765,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -3005,7 +3005,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -3026,7 +3026,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>

</xml_diff>